<commit_message>
SSDM-12286 Added support for packaging entity validation plugins and dynamic property plugins.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment-type.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment-type.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vkovtun/Work/Projects/openBIS/sissource/openbis/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33D902A-0A29-9141-AD04-34E2F8E4A37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141B454F-2FD7-6C40-B588-AB47C70E65F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1060" windowWidth="27340" windowHeight="16940" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
+    <workbookView xWindow="4540" yWindow="3520" windowWidth="27340" windowHeight="16940" xr2:uid="{75C30B8F-E590-0942-81AA-3FAD886CC976}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -107,18 +107,6 @@
     <t>DEFAULT_EXPERIMENT</t>
   </si>
   <si>
-    <t xml:space="preserve">def getRenderedProperty(entity, property):
-    value = entity.property(property)
-    if value is not None:
-        return value.renderedValue()
-def validate(entity, isNew):
-    start_date = getRenderedProperty(entity, "START_DATE")
-    end_date = getRenderedProperty(entity, "END_DATE")
-    if start_date is not None and end_date is not None and start_date &gt; end_date:
-        return "End date cannot be before start date!"
-</t>
-  </si>
-  <si>
     <t>$DEFAULT_OBJECT_TYPE</t>
   </si>
   <si>
@@ -144,6 +132,9 @@
   </si>
   <si>
     <t>Vocabulary code</t>
+  </si>
+  <si>
+    <t>test.py</t>
   </si>
 </sst>
 </file>
@@ -509,7 +500,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,7 +529,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -564,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>11</v>
@@ -616,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -628,7 +619,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -637,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>5</v>
@@ -651,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>15</v>
@@ -661,7 +652,7 @@
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>19</v>
@@ -670,7 +661,7 @@
         <v>5</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>20</v>
@@ -684,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>15</v>
@@ -694,7 +685,7 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>21</v>
@@ -703,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>5</v>

</xml_diff>